<commit_message>
payment reminder label and allowing only orders with Natuurlik Free Delivery on the app
</commit_message>
<xml_diff>
--- a/NatuurlikBase/NatuurlikBase/wwwroot/Uploads/Book1(1).xlsx
+++ b/NatuurlikBase/NatuurlikBase/wwwroot/Uploads/Book1(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D550B-F571-48BD-AFAD-0AE4D78998D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2084EF-6A52-4ECD-9CF1-0987FC5B2230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="2610" windowWidth="21600" windowHeight="11835" xr2:uid="{0F397AEF-E452-493C-A3FB-B550E9DF8F35}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15300" windowHeight="7785" xr2:uid="{0F397AEF-E452-493C-A3FB-B550E9DF8F35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>8 days</t>
+  </si>
+  <si>
+    <t>30 days</t>
   </si>
 </sst>
 </file>
@@ -124,8 +127,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{29505B2A-EFBD-4B60-A91C-B85B754B4C38}" name="Id"/>
     <tableColumn id="2" xr3:uid="{45663EE1-61F8-47B3-9F02-2D44639F9FEE}" name="Days"/>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B53E2A1-97C5-4C77-B2EF-6BD6BFD587A1}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +581,20 @@
         <v>22</v>
       </c>
       <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>